<commit_message>
changing example 4 to fit the new templat
</commit_message>
<xml_diff>
--- a/SampleApp/GraphTemplate.xlsx
+++ b/SampleApp/GraphTemplate.xlsx
@@ -1,41 +1,304 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\EPPlus-master\SampleApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D172F44D-8471-4668-B9A6-3AA0FE319AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rates Sample" sheetId="1" r:id="rId1"/>
+    <sheet name="CTRLQ" sheetId="2" r:id="rId1"/>
+    <sheet name="Rates Sample" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+  <si>
+    <t>ביצוע ע"י QC/QA</t>
+  </si>
+  <si>
+    <t>מס' סידורי</t>
+  </si>
+  <si>
+    <t>רשימת תיוג</t>
+  </si>
+  <si>
+    <t>תאריך הבדיקה</t>
+  </si>
+  <si>
+    <t>מבנה: כביש\ציר \רמפה\ מדרכה\ אי תנועה...</t>
+  </si>
+  <si>
+    <t>מחתך</t>
+  </si>
+  <si>
+    <t>עד חתך</t>
+  </si>
+  <si>
+    <t>צד</t>
+  </si>
+  <si>
+    <t>שטח</t>
+  </si>
+  <si>
+    <t>שכבה מס'</t>
+  </si>
+  <si>
+    <t>עובי השכבה</t>
+  </si>
+  <si>
+    <t>סוג עבודה</t>
+  </si>
+  <si>
+    <t>תאור החומר</t>
+  </si>
+  <si>
+    <t>מיון החומר</t>
+  </si>
+  <si>
+    <t>מקור החומר</t>
+  </si>
+  <si>
+    <t>הידוק רגיל  (מעברי מכבש)</t>
+  </si>
+  <si>
+    <t>מעמד</t>
+  </si>
+  <si>
+    <t>מס' תעודת בדיקה צפיפות /  רטיבות שדה</t>
+  </si>
+  <si>
+    <t>הידוק מבוקר (צפיפות מד גרעיני)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> מנת בדיקה (חרוט חול / שלבי)</t>
+  </si>
+  <si>
+    <t>מדידה</t>
+  </si>
+  <si>
+    <t>מספר תעודת בדיקת אפיון - 100%</t>
+  </si>
+  <si>
+    <t>FWD</t>
+  </si>
+  <si>
+    <t>צפיפות מחושבת (ק"ג/מ"ק)</t>
+  </si>
+  <si>
+    <t>צפיפות סטטיסטיקה</t>
+  </si>
+  <si>
+    <t>בדיקה חוזרת לתעודה / תעודת תיוק מס'</t>
+  </si>
+  <si>
+    <t>מתאריך</t>
+  </si>
+  <si>
+    <t>הערות</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>מס'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">תאריך </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>מ"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>ר</t>
+    </r>
+  </si>
+  <si>
+    <t>ס"מ</t>
+  </si>
+  <si>
+    <t>קרקע יסוד / מילוי / חפירה</t>
+  </si>
+  <si>
+    <t>AASHTO</t>
+  </si>
+  <si>
+    <t>כמות  מעברי מכבש</t>
+  </si>
+  <si>
+    <t>OK/NC</t>
+  </si>
+  <si>
+    <t>כמות נקודות בדיקה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">כמות נקודות  </t>
+  </si>
+  <si>
+    <t>תאריך</t>
+  </si>
+  <si>
+    <t>מספר תעודה</t>
+  </si>
+  <si>
+    <t>גבול תחתון (%)</t>
+  </si>
+  <si>
+    <t>גבול עליון (%)</t>
+  </si>
+  <si>
+    <t>ממוצע (%)</t>
+  </si>
+  <si>
+    <t>מס' רשימת תיוג NC</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>51.02.067</t>
+  </si>
+  <si>
+    <t>רמפה NW סופי</t>
+  </si>
+  <si>
+    <t>1935</t>
+  </si>
+  <si>
+    <t>4630</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>מילוי</t>
+  </si>
+  <si>
+    <t>חול צהוב</t>
+  </si>
+  <si>
+    <t>A-3</t>
+  </si>
+  <si>
+    <t>מקומי</t>
+  </si>
+  <si>
+    <t>516389</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1005175</t>
+  </si>
+  <si>
+    <t>1775</t>
+  </si>
+  <si>
+    <t>98.4</t>
+  </si>
+  <si>
+    <t>99.1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="[$-1040D]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="David"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -43,27 +306,109 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="sv-SE"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -81,12 +426,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -105,10 +452,19 @@
             <c:numRef>
               <c:f>'Rates Sample'!$A$22:$A$26</c:f>
               <c:numCache>
-                <c:formatCode>yyyy/mm/dd</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39783</c:v>
+                  <c:v>12212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -122,9 +478,27 @@
                 <c:pt idx="0" formatCode="#,##0.0000">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B917-41D6-8696-3210220A0F53}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -139,10 +513,19 @@
             <c:numRef>
               <c:f>'Rates Sample'!$A$22:$A$26</c:f>
               <c:numCache>
-                <c:formatCode>yyyy/mm/dd</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39783</c:v>
+                  <c:v>12212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -156,6 +539,12 @@
               </c:pt>
             </c:numLit>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B917-41D6-8696-3210220A0F53}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -170,10 +559,19 @@
             <c:numRef>
               <c:f>'Rates Sample'!$A$22:$A$26</c:f>
               <c:numCache>
-                <c:formatCode>yyyy/mm/dd</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39783</c:v>
+                  <c:v>12212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -187,32 +585,54 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B917-41D6-8696-3210220A0F53}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="165312384"/>
         <c:axId val="165313920"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="165312384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:crossAx val="165313920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="165313920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="165312384"/>
         <c:crosses val="autoZero"/>
@@ -221,10 +641,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -238,20 +659,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1026" name="SampleChart"/>
+        <xdr:cNvPr id="1026" name="SampleChart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -272,7 +699,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -314,7 +741,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,9 +773,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,6 +825,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -555,33 +1018,380 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A21:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB20375-F0D5-49D4-940E-9BCA24C6DE90}">
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:35" s="8" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="11">
+        <v>43140</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="W3" s="11">
+        <v>43139</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AC1:AF1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A21:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>39783</v>
+        <v>12212</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>